<commit_message>
Fixed default column behavior Issue of InsertData returns invalid Range Setting a cell to an empty string will convert the datatype to Text. Rich text composed only of spaces now work.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/ColumnCells.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/ColumnCells.xlsx
@@ -393,10 +393,9 @@
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="2" max="16384" width="9.850625" style="0" customWidth="1"/>
-    <x:col min="1" max="1" width="9.850625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">

</xml_diff>

<commit_message>
Removed .ClearStyles, use .Clear(XLClearOptions.Formats) instead Improved performance Dramatically reduced memory consumption
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/ColumnCells.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/ColumnCells.xlsx
@@ -70,7 +70,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="5">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -80,14 +80,8 @@
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="5">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -98,14 +92,6 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -413,32 +399,32 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">
-      <x:c r="A1" s="3" t="s"/>
-      <x:c r="B1" s="3" t="s"/>
+      <x:c r="A1" s="1" t="s"/>
+      <x:c r="B1" s="1" t="s"/>
     </x:row>
     <x:row r="2" spans="1:2">
-      <x:c r="A2" s="4" t="s"/>
-      <x:c r="B2" s="4" t="s"/>
+      <x:c r="A2" s="2" t="s"/>
+      <x:c r="B2" s="2" t="s"/>
     </x:row>
     <x:row r="3" spans="1:2">
-      <x:c r="A3" s="3" t="s"/>
-      <x:c r="B3" s="3" t="s"/>
+      <x:c r="A3" s="1" t="s"/>
+      <x:c r="B3" s="1" t="s"/>
     </x:row>
     <x:row r="5" spans="1:2">
-      <x:c r="A5" s="3" t="s"/>
-      <x:c r="B5" s="3" t="s"/>
+      <x:c r="A5" s="1" t="s"/>
+      <x:c r="B5" s="1" t="s"/>
     </x:row>
     <x:row r="6" spans="1:2">
-      <x:c r="A6" s="3" t="s"/>
-      <x:c r="B6" s="3" t="s"/>
+      <x:c r="A6" s="1" t="s"/>
+      <x:c r="B6" s="1" t="s"/>
     </x:row>
     <x:row r="8" spans="1:2">
-      <x:c r="A8" s="4" t="s"/>
-      <x:c r="B8" s="4" t="s"/>
+      <x:c r="A8" s="2" t="s"/>
+      <x:c r="B8" s="2" t="s"/>
     </x:row>
     <x:row r="9" spans="1:2">
-      <x:c r="A9" s="4" t="s"/>
-      <x:c r="B9" s="4" t="s"/>
+      <x:c r="A9" s="2" t="s"/>
+      <x:c r="B9" s="2" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Headers and Footer now keep their images when they're not modified.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/ColumnCells.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/ColumnCells.xlsx
@@ -430,14 +430,7 @@
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter differentOddEven="1" differentFirst="1" scaleWithDoc="1" alignWithMargins="1">
-    <x:oddHeader/>
-    <x:oddFooter/>
-    <x:evenHeader/>
-    <x:evenFooter/>
-    <x:firstHeader/>
-    <x:firstFooter/>
-  </x:headerFooter>
+  <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>